<commit_message>
Partial debug of general beamline parser
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-LsrDrvn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EEE769-D751-AF43-893B-FEBEDCDAFD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BC4DAE-1FDF-6048-9032-3B9B244A5E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>Parameter</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Mode</t>
-  </si>
-  <si>
     <t>SourceMode</t>
   </si>
   <si>
@@ -66,12 +63,6 @@
     <t>MeV</t>
   </si>
   <si>
-    <t>Sigma x</t>
-  </si>
-  <si>
-    <t>Sigma y</t>
-  </si>
-  <si>
     <t>SigmaX</t>
   </si>
   <si>
@@ -93,15 +84,9 @@
     <t>Length</t>
   </si>
   <si>
-    <t>Drift1Length</t>
-  </si>
-  <si>
     <t>Length of first, compensated, drift</t>
   </si>
   <si>
-    <t>Drift2Length</t>
-  </si>
-  <si>
     <t>Circular</t>
   </si>
   <si>
@@ -114,33 +99,15 @@
     <t>Aperture</t>
   </si>
   <si>
-    <t>Radius1</t>
-  </si>
-  <si>
-    <t>Radius2</t>
-  </si>
-  <si>
-    <t>Minimum cos theta</t>
-  </si>
-  <si>
     <t>MinCTheta</t>
   </si>
   <si>
-    <t>Minimum energy</t>
-  </si>
-  <si>
-    <t>Maximum energy</t>
-  </si>
-  <si>
     <t>Minimum of energy distribution</t>
   </si>
   <si>
     <t>Maximum theta for flat cos theta</t>
   </si>
   <si>
-    <t>Number of points</t>
-  </si>
-  <si>
     <t>Emin</t>
   </si>
   <si>
@@ -166,6 +133,18 @@
   </si>
   <si>
     <t>LhARA</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Parameterised TNSA</t>
+  </si>
+  <si>
+    <t>Interface</t>
   </si>
 </sst>
 </file>
@@ -216,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -332,11 +311,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -350,6 +353,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,16 +674,16 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
@@ -692,11 +699,11 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -713,10 +720,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>1</v>
@@ -725,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -735,22 +742,22 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F3" s="10">
         <v>15</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="10"/>
     </row>
@@ -765,17 +772,17 @@
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -789,19 +796,19 @@
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" s="6">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -815,19 +822,19 @@
         <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -841,19 +848,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -867,19 +874,19 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F8" s="6">
         <v>25</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -893,145 +900,141 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F9" s="6">
         <v>1000</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="7">
         <v>0.998</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
-        <v>36</v>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="A11" s="12">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="12">
         <v>0.05</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>23</v>
+      <c r="G11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>1</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>8</v>
+      <c r="B12" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F12" s="6">
         <v>2E-3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>1</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>8</v>
+      <c r="B13" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F13" s="6">
         <v>0.05</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>8</v>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F14" s="7">
         <v>2.8700000000000002E-3</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begin to build stage 1 LhARA lattice
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-LsrDrvn.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB3334-BB1E-094A-B4AE-9E5B3B484280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E59B91-0A9E-AE49-BE6B-A925C4FF94D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
   <si>
     <t>Parameter</t>
   </si>
@@ -148,6 +159,36 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>Capture</t>
+  </si>
+  <si>
+    <t>Drift to solenoid</t>
+  </si>
+  <si>
+    <t>Solenoid</t>
+  </si>
+  <si>
+    <t>Length of solenoid</t>
+  </si>
+  <si>
+    <t>Length, strength</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>ks</t>
+  </si>
+  <si>
+    <t>rad/m</t>
+  </si>
+  <si>
+    <t>Drift out of solenoid</t>
+  </si>
+  <si>
+    <t>Drift to next solenoid</t>
   </si>
 </sst>
 </file>
@@ -198,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -338,11 +379,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -360,6 +410,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,10 +738,10 @@
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1040,6 +1093,204 @@
         <v>22</v>
       </c>
     </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
+        <v>1</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>1</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17">
+        <f>2.4916949087545</f>
+        <v>2.4916949087544999</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>1</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18">
+        <v>0.15</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>1</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>0.15</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <v>1</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <v>1</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21">
+        <v>1.0187472612650501</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <v>1</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Add CylindricalRFCavity and do bug fix for adding s for dipole in addBeamLine
</commit_message>
<xml_diff>
--- a/11-Parameters/LhARABeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/LhARABeamLine-Params-LsrDrvn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7E7FDC-5378-F24C-AA90-A6C027783301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B598E7C-2C31-4B43-A0B3-35468DE1D49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="640" windowWidth="21660" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="640" windowWidth="21660" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LhARABeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="80">
   <si>
     <t>Parameter</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Energy selection</t>
   </si>
   <si>
-    <t>Space for first cavity, modelled as drift</t>
-  </si>
-  <si>
     <t>Drift to energy-selection collimator</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
   </si>
   <si>
     <t>Space for energy-selection collimator?</t>
-  </si>
-  <si>
-    <t>Space for second cavity, modelled as drift</t>
   </si>
   <si>
     <t>Matching</t>
@@ -258,6 +252,42 @@
   </si>
   <si>
     <t>Mother volume radius</t>
+  </si>
+  <si>
+    <t>Drift before first cavity</t>
+  </si>
+  <si>
+    <t>Drift after first cavity</t>
+  </si>
+  <si>
+    <t>Cavity</t>
+  </si>
+  <si>
+    <t>Cylindrical</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>MV/m</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Phase of reference particle</t>
+  </si>
+  <si>
+    <t>Drift before second cavity</t>
+  </si>
+  <si>
+    <t>Drift after second cavity</t>
   </si>
 </sst>
 </file>
@@ -706,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,10 +837,10 @@
         <v>32</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F4" s="9">
         <v>0.5</v>
@@ -1312,13 +1342,14 @@
         <v>18</v>
       </c>
       <c r="F24" s="4">
-        <v>0.5</v>
+        <f>(0.5-0.132433454701889)/2</f>
+        <v>0.1837832726490555</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1329,20 +1360,22 @@
         <v>51</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E25" s="5" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F25" s="5">
-        <v>0.15</v>
+        <v>5</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1353,21 +1386,23 @@
         <v>51</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="F26" s="5">
-        <v>0.85699999999999998</v>
+        <v>200</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
@@ -1377,21 +1412,23 @@
         <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="F27" s="5">
-        <v>1.4485646330252</v>
+        <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
@@ -1408,13 +1445,14 @@
         <v>18</v>
       </c>
       <c r="F28" s="5">
-        <v>0.15</v>
+        <f>(0.5-0.132433454701889)/2</f>
+        <v>0.1837832726490555</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1432,13 +1470,13 @@
         <v>18</v>
       </c>
       <c r="F29" s="5">
-        <v>1.7709999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1449,21 +1487,21 @@
         <v>51</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E30" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F30" s="5">
-        <v>5.0000000000000001E-3</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
@@ -1473,23 +1511,21 @@
         <v>51</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F31" s="5">
-        <v>2.5000000000000001E-3</v>
+        <v>1.4485646330252</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
@@ -1506,13 +1542,13 @@
         <v>18</v>
       </c>
       <c r="F32" s="5">
-        <v>5.0000000000000001E-3</v>
+        <v>0.15</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1530,12 +1566,14 @@
         <v>18</v>
       </c>
       <c r="F33" s="5">
-        <v>6.4610000000000001E-2</v>
+        <v>1.7709999999999999</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
@@ -1552,12 +1590,14 @@
         <v>18</v>
       </c>
       <c r="F34" s="5">
-        <v>0.13539000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
@@ -1567,20 +1607,22 @@
         <v>51</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="E35" s="5" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F35" s="5">
-        <v>0.01</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1598,106 +1640,102 @@
         <v>18</v>
       </c>
       <c r="F36" s="5">
-        <v>5.4600000000000003E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H36" s="5"/>
+      <c r="H36" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="5">
+        <v>1</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="C37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="5">
+        <v>6.4610000000000001E-2</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>1</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="A38" s="5">
+        <v>1</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0.13539000000000001</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>1</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F39" s="5">
-        <v>0.85699999999999998</v>
+        <v>0.01</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="5"/>
+      <c r="H39" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F40" s="5">
-        <v>1.7888589662779599</v>
+        <v>5.4600000000000003E-2</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H40" s="5"/>
     </row>
@@ -1706,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>17</v>
@@ -1716,13 +1754,14 @@
         <v>18</v>
       </c>
       <c r="F41" s="5">
-        <v>0.15</v>
+        <f>(0.5-0.132433454701889)/2</f>
+        <v>0.1837832726490555</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1730,45 +1769,51 @@
         <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E42" s="5" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="F42" s="5">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E43" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="F43" s="5">
-        <v>0.15</v>
+        <v>200</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1776,71 +1821,74 @@
         <v>1</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F44" s="5">
-        <v>0.85699999999999998</v>
+        <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>1</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F45" s="5">
-        <v>1.60433994066042</v>
+        <f>(0.5-0.132433454701889)/2</f>
+        <v>0.1837832726490555</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H45" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
-        <v>1</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" s="5">
+      <c r="A46" s="4">
+        <v>1</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="4">
         <v>0.15</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>49</v>
+      <c r="G46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1848,17 +1896,19 @@
         <v>1</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E47" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F47" s="5">
-        <v>2.5</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>14</v>
@@ -1870,70 +1920,68 @@
         <v>1</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E48" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F48" s="5">
-        <v>0.15</v>
+        <v>1.7888589662779599</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>1</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F49" s="5">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H49" s="5"/>
+      <c r="H49" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>1</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F50" s="5">
-        <v>1.2448140165275099</v>
+        <v>0.3</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H50" s="5"/>
     </row>
@@ -1942,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>17</v>
@@ -1958,7 +2006,7 @@
         <v>14</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1966,17 +2014,19 @@
         <v>1</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E52" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F52" s="5">
-        <v>0.3</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>14</v>
@@ -1988,95 +2038,93 @@
         <v>1</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E53" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F53" s="5">
-        <v>0.15</v>
+        <v>1.60433994066042</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>1</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F54" s="5">
-        <v>0.85699999999999998</v>
+        <v>0.15</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H54" s="5"/>
+      <c r="H54" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>1</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D55" s="5"/>
       <c r="E55" s="5" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F55" s="5">
-        <v>1.1659674896013299</v>
+        <v>2.5</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
-        <v>1</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F56" s="3">
+      <c r="A56" s="5">
+        <v>1</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="5">
         <v>0.15</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>49</v>
+      <c r="G56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2084,17 +2132,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E57" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F57" s="5">
-        <v>0.2</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>14</v>
@@ -2106,22 +2156,22 @@
         <v>1</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F58" s="5">
-        <v>0.8</v>
+        <v>1.2448140165275099</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="H58" s="5"/>
     </row>
@@ -2130,31 +2180,31 @@
         <v>1</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>67</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="F59" s="5">
-        <v>45</v>
+        <v>0.15</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H59" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>1</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>17</v>
@@ -2164,7 +2214,7 @@
         <v>18</v>
       </c>
       <c r="F60" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>14</v>
@@ -2176,42 +2226,46 @@
         <v>1</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F61" s="5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H61" s="5"/>
-    </row>
-    <row r="62" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="H61" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>1</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D62" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E62" s="5" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="F62" s="5">
-        <v>22.544</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="H62" s="5"/>
     </row>
@@ -2220,64 +2274,68 @@
         <v>1</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E63" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F63" s="5">
-        <v>0.4</v>
+        <v>1.1659674896013299</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="5">
-        <v>1</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H64" s="5"/>
-    </row>
-    <row r="65" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>1</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>1</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="F65" s="5">
-        <v>31.376799999999999</v>
+        <v>0.2</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="H65" s="5"/>
     </row>
@@ -2286,17 +2344,19 @@
         <v>1</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D66" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="E66" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="5">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>14</v>
@@ -2308,42 +2368,44 @@
         <v>1</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="F67" s="5">
-        <v>0.1</v>
+        <v>45</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
         <v>1</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="F68" s="5">
-        <v>31.5123</v>
+        <v>0.2</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="H68" s="5"/>
     </row>
@@ -2352,245 +2414,242 @@
         <v>1</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F69" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
+        <v>1</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F70" s="5">
+        <v>22.544</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>1</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
+        <v>1</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A73" s="5">
+        <v>1</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F73" s="5">
+        <v>31.376799999999999</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>1</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="5">
+        <v>1</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A76" s="5">
+        <v>1</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F76" s="5">
+        <v>31.5123</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="5">
+        <v>1</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="5">
         <f>0.2-0.005</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="G69" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H69" s="5"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="5">
-        <v>1</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70" s="5">
+      <c r="G77" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="5">
+        <v>1</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" s="5">
         <v>0.01</v>
       </c>
-      <c r="G70" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" s="5"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="5">
-        <v>1</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F71" s="5">
+      <c r="G78" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="5">
+        <v>1</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="5">
         <f>0.2-0.005</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="G71" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" s="5"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="5">
-        <v>1</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F72" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H72" s="5"/>
-    </row>
-    <row r="73" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A73" s="5">
-        <v>1</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F73" s="5">
-        <f>F68</f>
-        <v>31.5123</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H73" s="5"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="5">
-        <v>1</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F74" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H74" s="5"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="5">
-        <v>1</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F75" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H75" s="5"/>
-    </row>
-    <row r="76" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A76" s="5">
-        <v>1</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F76" s="5">
-        <f>F65</f>
-        <v>31.376799999999999</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H76" s="5"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="5">
-        <v>1</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F77" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H77" s="5"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="5">
-        <v>1</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F78" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H78" s="5"/>
-    </row>
-    <row r="79" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A79" s="5">
-        <v>1</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F79" s="5">
-        <f>F62</f>
-        <v>22.544</v>
-      </c>
       <c r="G79" s="5" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="H79" s="5"/>
     </row>
@@ -2599,44 +2658,43 @@
         <v>1</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F80" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H80" s="5"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <v>1</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D81" s="5"/>
       <c r="E81" s="5" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="F81" s="5">
-        <v>0.8</v>
+        <f>F76</f>
+        <v>31.5123</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="H81" s="5"/>
     </row>
@@ -2645,22 +2703,20 @@
         <v>1</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>67</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D82" s="5"/>
       <c r="E82" s="5" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="F82" s="5">
-        <v>45</v>
+        <v>0.2</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="H82" s="5"/>
     </row>
@@ -2669,44 +2725,226 @@
         <v>1</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F83" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A84" s="5">
+        <v>1</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F84" s="5">
+        <f>F73</f>
+        <v>31.376799999999999</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="5">
+        <v>1</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
+        <v>1</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A87" s="5">
+        <v>1</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F87" s="5">
+        <f>F70</f>
+        <v>22.544</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <v>1</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="5">
         <v>0.2</v>
       </c>
-      <c r="G83" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H83" s="5"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="3">
-        <v>1</v>
-      </c>
-      <c r="B84" s="3" t="s">
+      <c r="G88" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="5">
+        <v>1</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F89" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>1</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F84" s="3">
+      <c r="F90" s="5">
+        <v>45</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
+        <v>1</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F91" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="3">
+        <v>1</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92" s="3">
         <v>2</v>
       </c>
-      <c r="G84" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H84" s="3"/>
+      <c r="G92" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>